<commit_message>
Signing WBA - Harun
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash Learning Materials\2019 - S2\FIT2099\Assignment Project\Design Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/SEM2/FIT2099/Assignemnt/project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68627605-6F51-43CA-9A92-9509F6026482}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4347DD27-D977-C64B-B5EF-72414F296CC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -74,13 +74,16 @@
   </si>
   <si>
     <t>Yes - Sara</t>
+  </si>
+  <si>
+    <t>YES - Harun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -352,19 +355,19 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="28">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -398,7 +401,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="13">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -412,7 +415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -423,7 +426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -434,18 +437,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="28">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13"/>
+    <row r="8" spans="1:27" ht="13">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -459,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="13">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -471,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -482,7 +488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -493,7 +499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="13">
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -504,7 +510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="26" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Signed WBA for assignment 2
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/SEM2/FIT2099/Assignemnt/project/Design Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash Learning Materials\2019 - S2\FIT2099\Assignment Project\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4347DD27-D977-C64B-B5EF-72414F296CC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3369B1E6-F2D1-4425-8CBD-C633F5C68F2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -352,22 +352,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="28">
+    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -401,7 +401,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="13">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -415,7 +415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="13">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -426,7 +426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="13">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -437,12 +437,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="28">
+    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="13">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -450,8 +450,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="13"/>
-    <row r="8" spans="1:27" ht="13">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -465,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="13">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -477,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -488,7 +488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -499,7 +499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="13">
+    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -510,9 +510,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="26" customHeight="1">
+    <row r="13" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Signed WBA for Assignment 2 - Harun
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash Learning Materials\2019 - S2\FIT2099\Assignment Project\Design Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/SEM2/FIT2099/Assignemnt/project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3369B1E6-F2D1-4425-8CBD-C633F5C68F2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56A91DA-F93C-AC43-B8E2-0101626208B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -355,19 +355,19 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="28">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -401,7 +401,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="13">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -415,7 +415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -426,7 +426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -437,12 +437,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="28">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -450,8 +450,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13"/>
+    <row r="8" spans="1:27" ht="13">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -465,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="13">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -477,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -488,7 +488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -499,7 +499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="13">
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -510,12 +510,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="26" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updated WBA for assignment 2 and signed
WBA for assignment 2 has been broken down into smaller and more specific tasks
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/SEM2/FIT2099/Assignemnt/project/Design Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash Learning Materials\2019 - S2\FIT2099\Assignment Project\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56A91DA-F93C-AC43-B8E2-0101626208B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943BABB9-CDFE-4817-AD02-5D716C51E669}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -46,24 +46,12 @@
     <t>ASSIGNMENT 2</t>
   </si>
   <si>
-    <t>Growing plants</t>
-  </si>
-  <si>
     <t>Sara</t>
   </si>
   <si>
-    <t>Hungry dinosaurs</t>
-  </si>
-  <si>
     <t>Baby dinosaurs</t>
   </si>
   <si>
-    <t>Buying and selling</t>
-  </si>
-  <si>
-    <t>Velociraptors</t>
-  </si>
-  <si>
     <t>Harun</t>
   </si>
   <si>
@@ -77,13 +65,43 @@
   </si>
   <si>
     <t>YES - Harun</t>
+  </si>
+  <si>
+    <t>Grow new tree</t>
+  </si>
+  <si>
+    <t>Grow new grass</t>
+  </si>
+  <si>
+    <t>Dinosaur class + species subclasses</t>
+  </si>
+  <si>
+    <t>BuyAction</t>
+  </si>
+  <si>
+    <t>SellAction</t>
+  </si>
+  <si>
+    <t>PlaceTagAction</t>
+  </si>
+  <si>
+    <t>FeedAction</t>
+  </si>
+  <si>
+    <t>EatAction</t>
+  </si>
+  <si>
+    <t>SeekFoodBehaviour</t>
+  </si>
+  <si>
+    <t>Dinosaurs laying egg and dying</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,6 +120,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -134,6 +165,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,22 +385,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="28">
+    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -401,129 +434,192 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="13">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="28">
-      <c r="A5" s="1" t="s">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="13">
-      <c r="A6" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="13"/>
-    <row r="8" spans="1:27" ht="13">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="13">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="B11" s="3" t="s">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="13">
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="26" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signed Assignment 2 WBA Agreement - Harun
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Monash Learning Materials\2019 - S2\FIT2099\Assignment Project\Design Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/SEM2/FIT2099/Assignemnt/project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943BABB9-CDFE-4817-AD02-5D716C51E669}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636E823C-A03D-3043-9E8E-69917925F2AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -101,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -388,19 +388,19 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="28">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -434,7 +434,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="13">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -448,7 +448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -459,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -470,12 +470,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="28">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -483,8 +483,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13"/>
+    <row r="8" spans="1:27" ht="13">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -498,7 +498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="13">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -520,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -531,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="13">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -542,7 +542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="26" customHeight="1">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -564,7 +564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -586,7 +586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -597,7 +597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -608,12 +608,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Update WBA for assignment 3
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{82D76C21-DCCF-42D2-848E-1DB71DD80CD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saratran/Documents/Monash Learning materials/2019 - S2/FIT2099/Assignment project/Design Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54960D11-1944-1049-A274-EC9D667F3766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28830" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
   <si>
     <t>Task/Deliverable</t>
   </si>
@@ -91,13 +95,41 @@
   </si>
   <si>
     <t>Dinosaurs laying egg and dying</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT 3</t>
+  </si>
+  <si>
+    <t>Add new map</t>
+  </si>
+  <si>
+    <t>Add Water (Ground)</t>
+  </si>
+  <si>
+    <t>Add Reeds growing and Fish spawning</t>
+  </si>
+  <si>
+    <t>T-Rex</t>
+  </si>
+  <si>
+    <t>Quit and Gameover</t>
+  </si>
+  <si>
+    <t>Pteanodons:
+- Flying over Land and Water
+- Move up to 2 squares per turn --&gt; need to modify WanderBehaviour</t>
+  </si>
+  <si>
+    <t>Plesiosaurs:
+- marine egg hatching
+- food preference --&gt; need to modify SeekFoodBehaviour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -130,6 +162,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -157,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -170,6 +208,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,22 +430,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="28">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -437,7 +479,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="13">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -451,7 +493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -462,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -473,12 +515,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="28">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -486,8 +528,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13"/>
+    <row r="8" spans="1:27" ht="13">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -501,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="13">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -512,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -523,7 +565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -534,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="13">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -545,7 +587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="26" customHeight="1">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -556,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -567,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -578,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -589,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -600,7 +642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -611,16 +653,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="56">
+      <c r="B27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="56">
+      <c r="B28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28">
+      <c r="A31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor fix for selling items
</commit_message>
<xml_diff>
--- a/Design Documents/Work Breakdown Agreement.xlsx
+++ b/Design Documents/Work Breakdown Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saratran/Documents/Monash Learning materials/2019 - S2/FIT2099/Assignment project/Design Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5761D3D4-4A13-6A4F-BB69-07DC03D67A76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756C20E5-86BB-A548-8B13-EAAC9C121ED4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,15 +136,18 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -430,7 +433,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -688,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="56">
       <c r="B26" s="9" t="s">
         <v>30</v>
       </c>

</xml_diff>